<commit_message>
Added 2020 results + clean up
</commit_message>
<xml_diff>
--- a/data/imputed/Congressional Election Results by State (2000 - 107th) IMPUTED.xlsx
+++ b/data/imputed/Congressional Election Results by State (2000 - 107th) IMPUTED.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11222"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/ushouse/data/imputed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B9E2D9-1294-8D45-8307-841DFDE03F4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C7968F-4722-1F49-BBB3-01ED948E3BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="500" windowWidth="24340" windowHeight="15540" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Election Results by State" sheetId="2" r:id="rId1"/>
     <sheet name="Uncontested Races" sheetId="4" r:id="rId2"/>
     <sheet name="Uncontested by State PIVOT" sheetId="6" r:id="rId3"/>
-    <sheet name="Assumptions" sheetId="8" r:id="rId4"/>
-    <sheet name="EXPORT" sheetId="9" r:id="rId5"/>
+    <sheet name="EXPORT" sheetId="9" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Election Results by State'!$A$2:$X$52</definedName>
@@ -25,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="195">
   <si>
     <t>Votes</t>
   </si>
@@ -603,9 +602,6 @@
   </si>
   <si>
     <t>SEAT_%</t>
-  </si>
-  <si>
-    <t>Super small # =</t>
   </si>
   <si>
     <t>STATE</t>
@@ -3465,7 +3461,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:F54" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="21">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -4290,10 +4286,10 @@
   <dimension ref="A1:X58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="X52" sqref="A1:X52"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8701,6 +8697,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A2:X52" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -16009,6 +16006,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A2:J94" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -17073,42 +17071,16 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B1" s="21">
-        <f>(1/100)/1000000</f>
-        <v>1E-8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D139691-7F93-3B44-B09F-7CDA2E004473}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -17119,34 +17091,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" t="s">
         <v>186</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>187</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>188</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>189</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>190</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>191</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>192</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>193</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>194</v>
-      </c>
-      <c r="J1" t="s">
-        <v>195</v>
       </c>
       <c r="K1" s="121" t="s">
         <v>183</v>
@@ -19056,6 +19028,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>